<commit_message>
Updated input files for inflow blocks.
Updated input data files to accommodate the inflow block functionality
</commit_message>
<xml_diff>
--- a/input_data/example_model.xlsx
+++ b/input_data/example_model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dsdennis\HOPE\Predicer\input_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{734092DA-7027-4E14-A19A-1DB00514F1D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{604BF146-86E9-496E-83C5-804CF812A978}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8964" tabRatio="796" firstSheet="11" activeTab="19" xr2:uid="{788BFBD1-D930-4535-8A91-D85C56924796}"/>
+    <workbookView xWindow="2232" yWindow="2232" windowWidth="17280" windowHeight="8964" tabRatio="796" firstSheet="10" activeTab="10" xr2:uid="{788BFBD1-D930-4535-8A91-D85C56924796}"/>
   </bookViews>
   <sheets>
     <sheet name="timeseries" sheetId="18" r:id="rId1"/>
@@ -23,17 +23,18 @@
     <sheet name="reserve_type" sheetId="13" r:id="rId8"/>
     <sheet name="cf" sheetId="7" r:id="rId9"/>
     <sheet name="inflow" sheetId="3" r:id="rId10"/>
-    <sheet name="price" sheetId="4" r:id="rId11"/>
-    <sheet name="markets" sheetId="5" r:id="rId12"/>
-    <sheet name="market_prices" sheetId="8" r:id="rId13"/>
-    <sheet name="balance_prices" sheetId="20" r:id="rId14"/>
-    <sheet name="risk" sheetId="17" r:id="rId15"/>
-    <sheet name="scenarios" sheetId="9" r:id="rId16"/>
-    <sheet name="fixed_ts" sheetId="11" r:id="rId17"/>
-    <sheet name="eff_ts" sheetId="12" r:id="rId18"/>
-    <sheet name="cap_ts" sheetId="16" r:id="rId19"/>
-    <sheet name="constraints" sheetId="14" r:id="rId20"/>
-    <sheet name="gen_constraint" sheetId="15" r:id="rId21"/>
+    <sheet name="inflow_blocks" sheetId="22" r:id="rId11"/>
+    <sheet name="price" sheetId="4" r:id="rId12"/>
+    <sheet name="markets" sheetId="5" r:id="rId13"/>
+    <sheet name="market_prices" sheetId="8" r:id="rId14"/>
+    <sheet name="balance_prices" sheetId="20" r:id="rId15"/>
+    <sheet name="risk" sheetId="17" r:id="rId16"/>
+    <sheet name="scenarios" sheetId="9" r:id="rId17"/>
+    <sheet name="fixed_ts" sheetId="11" r:id="rId18"/>
+    <sheet name="eff_ts" sheetId="12" r:id="rId19"/>
+    <sheet name="cap_ts" sheetId="16" r:id="rId20"/>
+    <sheet name="constraints" sheetId="14" r:id="rId21"/>
+    <sheet name="gen_constraint" sheetId="15" r:id="rId22"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -53,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="98">
   <si>
     <t>node</t>
   </si>
@@ -4484,6 +4485,98 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E44A96C9-CA4B-4735-AF1E-65BD86DB3657}">
+  <dimension ref="A1:F17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="6" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="8"/>
+      <c r="E2" s="8"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="C3" s="8"/>
+      <c r="E3" s="8"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="C4" s="8"/>
+      <c r="E4" s="8"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="C5" s="8"/>
+      <c r="E5" s="8"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+    </row>
+    <row r="17" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02307C1F-427B-487D-B703-EBF512D7AC27}">
   <dimension ref="A1:C25"/>
   <sheetViews>
@@ -4717,7 +4810,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3788A93-7501-4F5D-9E8F-38D329CC85EC}">
   <dimension ref="A1:K5"/>
   <sheetViews>
@@ -4884,7 +4977,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF6DDD9A-EF34-4108-8532-230729E9C708}">
   <dimension ref="A1:G11"/>
   <sheetViews>
@@ -5170,7 +5263,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{817FDE8F-BC70-48D0-8376-FB52E6946AF1}">
   <dimension ref="A1:E25"/>
   <sheetViews>
@@ -5474,7 +5567,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9314D326-256A-435C-AAE3-3517FA836EAE}">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -5516,7 +5609,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A87AD413-E614-48C1-80E1-F1E8236FCBC6}">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -5555,7 +5648,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31679CA5-0AA2-4F6F-8223-14BF74917F04}">
   <dimension ref="A1:B25"/>
   <sheetViews>
@@ -5729,7 +5822,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD670E02-665B-45B8-BC4E-9596D2C1BC55}">
   <dimension ref="A1:A25"/>
   <sheetViews>
@@ -5893,173 +5986,6 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7FEDBA5-B0F3-4E9D-9367-08D5F5FA8AEA}">
-  <dimension ref="A1:A25"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="19.33203125" style="8" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" s="8">
-        <f>IF(timeseries!A2&lt;&gt;"",timeseries!A2,"")</f>
-        <v>44671</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" s="8">
-        <f>IF(timeseries!A3&lt;&gt;"",timeseries!A3,"")</f>
-        <v>44671.041666666664</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" s="8">
-        <f>IF(timeseries!A4&lt;&gt;"",timeseries!A4,"")</f>
-        <v>44671.08333321759</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" s="8">
-        <f>IF(timeseries!A5&lt;&gt;"",timeseries!A5,"")</f>
-        <v>44671.124999826388</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" s="8">
-        <f>IF(timeseries!A6&lt;&gt;"",timeseries!A6,"")</f>
-        <v>44671.166666435187</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7" s="8">
-        <f>IF(timeseries!A7&lt;&gt;"",timeseries!A7,"")</f>
-        <v>44671.208333043978</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8" s="8">
-        <f>IF(timeseries!A8&lt;&gt;"",timeseries!A8,"")</f>
-        <v>44671.249999537038</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A9" s="8">
-        <f>IF(timeseries!A9&lt;&gt;"",timeseries!A9,"")</f>
-        <v>44671.291666087964</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A10" s="8">
-        <f>IF(timeseries!A10&lt;&gt;"",timeseries!A10,"")</f>
-        <v>44671.333332638889</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A11" s="8">
-        <f>IF(timeseries!A11&lt;&gt;"",timeseries!A11,"")</f>
-        <v>44671.374999189815</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A12" s="8" t="str">
-        <f>IF(timeseries!A12&lt;&gt;"",timeseries!A12,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A13" s="8" t="str">
-        <f>IF(timeseries!A13&lt;&gt;"",timeseries!A13,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A14" s="8" t="str">
-        <f>IF(timeseries!A14&lt;&gt;"",timeseries!A14,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A15" s="8" t="str">
-        <f>IF(timeseries!A15&lt;&gt;"",timeseries!A15,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A16" s="8" t="str">
-        <f>IF(timeseries!A16&lt;&gt;"",timeseries!A16,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" s="8" t="str">
-        <f>IF(timeseries!A17&lt;&gt;"",timeseries!A17,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" s="8" t="str">
-        <f>IF(timeseries!A18&lt;&gt;"",timeseries!A18,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" s="8" t="str">
-        <f>IF(timeseries!A19&lt;&gt;"",timeseries!A19,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20" s="8" t="str">
-        <f>IF(timeseries!A20&lt;&gt;"",timeseries!A20,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21" s="8" t="str">
-        <f>IF(timeseries!A21&lt;&gt;"",timeseries!A21,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A22" s="8" t="str">
-        <f>IF(timeseries!A22&lt;&gt;"",timeseries!A22,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A23" s="8" t="str">
-        <f>IF(timeseries!A23&lt;&gt;"",timeseries!A23,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A24" s="8" t="str">
-        <f>IF(timeseries!A24&lt;&gt;"",timeseries!A24,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A25" s="8" t="str">
-        <f>IF(timeseries!A25&lt;&gt;"",timeseries!A25,"")</f>
-        <v/>
-      </c>
-    </row>
-  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -6243,10 +6169,177 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7FEDBA5-B0F3-4E9D-9367-08D5F5FA8AEA}">
+  <dimension ref="A1:A25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="19.33203125" style="8" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" s="8">
+        <f>IF(timeseries!A2&lt;&gt;"",timeseries!A2,"")</f>
+        <v>44671</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" s="8">
+        <f>IF(timeseries!A3&lt;&gt;"",timeseries!A3,"")</f>
+        <v>44671.041666666664</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" s="8">
+        <f>IF(timeseries!A4&lt;&gt;"",timeseries!A4,"")</f>
+        <v>44671.08333321759</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" s="8">
+        <f>IF(timeseries!A5&lt;&gt;"",timeseries!A5,"")</f>
+        <v>44671.124999826388</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" s="8">
+        <f>IF(timeseries!A6&lt;&gt;"",timeseries!A6,"")</f>
+        <v>44671.166666435187</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" s="8">
+        <f>IF(timeseries!A7&lt;&gt;"",timeseries!A7,"")</f>
+        <v>44671.208333043978</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" s="8">
+        <f>IF(timeseries!A8&lt;&gt;"",timeseries!A8,"")</f>
+        <v>44671.249999537038</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" s="8">
+        <f>IF(timeseries!A9&lt;&gt;"",timeseries!A9,"")</f>
+        <v>44671.291666087964</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" s="8">
+        <f>IF(timeseries!A10&lt;&gt;"",timeseries!A10,"")</f>
+        <v>44671.333332638889</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" s="8">
+        <f>IF(timeseries!A11&lt;&gt;"",timeseries!A11,"")</f>
+        <v>44671.374999189815</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" s="8" t="str">
+        <f>IF(timeseries!A12&lt;&gt;"",timeseries!A12,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" s="8" t="str">
+        <f>IF(timeseries!A13&lt;&gt;"",timeseries!A13,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14" s="8" t="str">
+        <f>IF(timeseries!A14&lt;&gt;"",timeseries!A14,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15" s="8" t="str">
+        <f>IF(timeseries!A15&lt;&gt;"",timeseries!A15,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A16" s="8" t="str">
+        <f>IF(timeseries!A16&lt;&gt;"",timeseries!A16,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="8" t="str">
+        <f>IF(timeseries!A17&lt;&gt;"",timeseries!A17,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" s="8" t="str">
+        <f>IF(timeseries!A18&lt;&gt;"",timeseries!A18,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" s="8" t="str">
+        <f>IF(timeseries!A19&lt;&gt;"",timeseries!A19,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" s="8" t="str">
+        <f>IF(timeseries!A20&lt;&gt;"",timeseries!A20,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" s="8" t="str">
+        <f>IF(timeseries!A21&lt;&gt;"",timeseries!A21,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" s="8" t="str">
+        <f>IF(timeseries!A22&lt;&gt;"",timeseries!A22,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" s="8" t="str">
+        <f>IF(timeseries!A23&lt;&gt;"",timeseries!A23,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" s="8" t="str">
+        <f>IF(timeseries!A24&lt;&gt;"",timeseries!A24,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" s="8" t="str">
+        <f>IF(timeseries!A25&lt;&gt;"",timeseries!A25,"")</f>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5704FC51-737E-45F9-9A9E-85A96AFE5439}">
   <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -6296,7 +6389,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE12AB76-2BDA-4ACA-A128-8CFB9FB6C8F8}">
   <dimension ref="A1:G25"/>
   <sheetViews>

</xml_diff>

<commit_message>
Added and updated example models
Added and updated example models.
</commit_message>
<xml_diff>
--- a/input_data/example_model.xlsx
+++ b/input_data/example_model.xlsx
@@ -1,43 +1,44 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dsdennis\HOPE\Predicer\input_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{803D4E30-ECA5-4E7E-AABC-A727FC1AB654}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{926E3452-50C3-4EDF-B8AE-413606A4C241}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="796" activeTab="7" xr2:uid="{788BFBD1-D930-4535-8A91-D85C56924796}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="796" activeTab="1" xr2:uid="{788BFBD1-D930-4535-8A91-D85C56924796}"/>
   </bookViews>
   <sheets>
     <sheet name="timeseries" sheetId="18" r:id="rId1"/>
-    <sheet name="nodes" sheetId="1" r:id="rId2"/>
-    <sheet name="processes" sheetId="2" r:id="rId3"/>
-    <sheet name="groups" sheetId="21" r:id="rId4"/>
-    <sheet name="efficiencies" sheetId="10" r:id="rId5"/>
-    <sheet name="process_topology" sheetId="6" r:id="rId6"/>
-    <sheet name="node_history" sheetId="19" r:id="rId7"/>
-    <sheet name="node_delay" sheetId="25" r:id="rId8"/>
-    <sheet name="node_diffusion" sheetId="24" r:id="rId9"/>
-    <sheet name="reserve_type" sheetId="13" r:id="rId10"/>
-    <sheet name="cf" sheetId="7" r:id="rId11"/>
-    <sheet name="inflow" sheetId="3" r:id="rId12"/>
-    <sheet name="inflow_blocks" sheetId="22" r:id="rId13"/>
-    <sheet name="price" sheetId="4" r:id="rId14"/>
-    <sheet name="markets" sheetId="5" r:id="rId15"/>
-    <sheet name="reserve_realisation" sheetId="23" r:id="rId16"/>
-    <sheet name="market_prices" sheetId="8" r:id="rId17"/>
-    <sheet name="balance_prices" sheetId="20" r:id="rId18"/>
-    <sheet name="risk" sheetId="17" r:id="rId19"/>
-    <sheet name="scenarios" sheetId="9" r:id="rId20"/>
-    <sheet name="fixed_ts" sheetId="11" r:id="rId21"/>
-    <sheet name="eff_ts" sheetId="12" r:id="rId22"/>
-    <sheet name="cap_ts" sheetId="16" r:id="rId23"/>
-    <sheet name="constraints" sheetId="14" r:id="rId24"/>
-    <sheet name="gen_constraint" sheetId="15" r:id="rId25"/>
+    <sheet name="setup" sheetId="26" r:id="rId2"/>
+    <sheet name="nodes" sheetId="1" r:id="rId3"/>
+    <sheet name="processes" sheetId="2" r:id="rId4"/>
+    <sheet name="groups" sheetId="21" r:id="rId5"/>
+    <sheet name="efficiencies" sheetId="10" r:id="rId6"/>
+    <sheet name="process_topology" sheetId="6" r:id="rId7"/>
+    <sheet name="node_history" sheetId="19" r:id="rId8"/>
+    <sheet name="node_delay" sheetId="25" r:id="rId9"/>
+    <sheet name="node_diffusion" sheetId="24" r:id="rId10"/>
+    <sheet name="reserve_type" sheetId="13" r:id="rId11"/>
+    <sheet name="cf" sheetId="7" r:id="rId12"/>
+    <sheet name="inflow" sheetId="3" r:id="rId13"/>
+    <sheet name="inflow_blocks" sheetId="22" r:id="rId14"/>
+    <sheet name="price" sheetId="4" r:id="rId15"/>
+    <sheet name="markets" sheetId="5" r:id="rId16"/>
+    <sheet name="reserve_realisation" sheetId="23" r:id="rId17"/>
+    <sheet name="market_prices" sheetId="8" r:id="rId18"/>
+    <sheet name="balance_prices" sheetId="20" r:id="rId19"/>
+    <sheet name="risk" sheetId="17" r:id="rId20"/>
+    <sheet name="scenarios" sheetId="9" r:id="rId21"/>
+    <sheet name="fixed_ts" sheetId="11" r:id="rId22"/>
+    <sheet name="eff_ts" sheetId="12" r:id="rId23"/>
+    <sheet name="cap_ts" sheetId="16" r:id="rId24"/>
+    <sheet name="constraints" sheetId="14" r:id="rId25"/>
+    <sheet name="gen_constraint" sheetId="15" r:id="rId26"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -57,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="122">
   <si>
     <t>node</t>
   </si>
@@ -390,6 +391,39 @@
   </si>
   <si>
     <t>max_flow</t>
+  </si>
+  <si>
+    <t>initial_flow</t>
+  </si>
+  <si>
+    <t>initial_load</t>
+  </si>
+  <si>
+    <t>scenario_independent_online</t>
+  </si>
+  <si>
+    <t>scenario_independent_state</t>
+  </si>
+  <si>
+    <t>use_market_bids</t>
+  </si>
+  <si>
+    <t>use_reserves</t>
+  </si>
+  <si>
+    <t>use_reserve_realisation</t>
+  </si>
+  <si>
+    <t>use_node_dummy_variables</t>
+  </si>
+  <si>
+    <t>use_ramp_dummy_variables</t>
+  </si>
+  <si>
+    <t>common_timesteps</t>
+  </si>
+  <si>
+    <t>common_scenario_name</t>
   </si>
 </sst>
 </file>
@@ -4064,178 +4098,178 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
         <v>44671</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <v>44671.041666666664</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <v>44671.08333321759</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <v>44671.124999826388</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <v>44671.166666435187</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <v>44671.208333043978</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <v>44671.249999537038</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <v>44671.291666087964</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
         <v>44671.333332638889</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <v>44671.374999189815</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="8"/>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="8"/>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="8"/>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="8"/>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="8"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="8"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="8"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="8"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="8"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="8"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="8"/>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="8"/>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="8"/>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="8"/>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="8"/>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="8"/>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="8"/>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="8"/>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="8"/>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="8"/>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="8"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="8"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="8"/>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="8"/>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="8"/>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="8"/>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="8"/>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="8"/>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="8"/>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="8"/>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="8"/>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="8"/>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="8"/>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="8"/>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="8"/>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="8"/>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="8"/>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="8"/>
     </row>
   </sheetData>
@@ -4245,6 +4279,36 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8F1FEF7-A337-4ADD-8F2A-03D982D23844}">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.85546875" style="8" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0532F8A-0FB4-47AD-98A1-4065D3376432}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -4252,9 +4316,9 @@
       <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>30</v>
       </c>
@@ -4262,7 +4326,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>43</v>
       </c>
@@ -4275,7 +4339,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77A4637A-7829-48D6-AE54-2E654AB1A427}">
   <dimension ref="A1:L25"/>
   <sheetViews>
@@ -4283,15 +4347,15 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.33203125" style="8" customWidth="1"/>
-    <col min="2" max="5" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" style="8" customWidth="1"/>
+    <col min="2" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>25</v>
       </c>
@@ -4302,7 +4366,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
         <f>IF(timeseries!A2&lt;&gt;"",timeseries!A2,"")</f>
         <v>44671</v>
@@ -4316,7 +4380,7 @@
       <c r="F2" s="8"/>
       <c r="L2" s="8"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <f>IF(timeseries!A3&lt;&gt;"",timeseries!A3,"")</f>
         <v>44671.041666666664</v>
@@ -4328,7 +4392,7 @@
         <v>0.52</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <f>IF(timeseries!A4&lt;&gt;"",timeseries!A4,"")</f>
         <v>44671.08333321759</v>
@@ -4340,7 +4404,7 @@
         <v>0.56000000000000005</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <f>IF(timeseries!A5&lt;&gt;"",timeseries!A5,"")</f>
         <v>44671.124999826388</v>
@@ -4352,7 +4416,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <f>IF(timeseries!A6&lt;&gt;"",timeseries!A6,"")</f>
         <v>44671.166666435187</v>
@@ -4364,7 +4428,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <f>IF(timeseries!A7&lt;&gt;"",timeseries!A7,"")</f>
         <v>44671.208333043978</v>
@@ -4376,7 +4440,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <f>IF(timeseries!A8&lt;&gt;"",timeseries!A8,"")</f>
         <v>44671.249999537038</v>
@@ -4388,7 +4452,7 @@
         <v>0.39</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <f>IF(timeseries!A9&lt;&gt;"",timeseries!A9,"")</f>
         <v>44671.291666087964</v>
@@ -4400,7 +4464,7 @@
         <v>0.47</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
         <f>IF(timeseries!A10&lt;&gt;"",timeseries!A10,"")</f>
         <v>44671.333332638889</v>
@@ -4412,7 +4476,7 @@
         <v>0.39</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <f>IF(timeseries!A11&lt;&gt;"",timeseries!A11,"")</f>
         <v>44671.374999189815</v>
@@ -4424,85 +4488,85 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="str">
         <f>IF(timeseries!A12&lt;&gt;"",timeseries!A12,"")</f>
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="str">
         <f>IF(timeseries!A13&lt;&gt;"",timeseries!A13,"")</f>
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="str">
         <f>IF(timeseries!A14&lt;&gt;"",timeseries!A14,"")</f>
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="str">
         <f>IF(timeseries!A15&lt;&gt;"",timeseries!A15,"")</f>
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="str">
         <f>IF(timeseries!A16&lt;&gt;"",timeseries!A16,"")</f>
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="str">
         <f>IF(timeseries!A17&lt;&gt;"",timeseries!A17,"")</f>
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="str">
         <f>IF(timeseries!A18&lt;&gt;"",timeseries!A18,"")</f>
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="str">
         <f>IF(timeseries!A19&lt;&gt;"",timeseries!A19,"")</f>
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="str">
         <f>IF(timeseries!A20&lt;&gt;"",timeseries!A20,"")</f>
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="str">
         <f>IF(timeseries!A21&lt;&gt;"",timeseries!A21,"")</f>
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="str">
         <f>IF(timeseries!A22&lt;&gt;"",timeseries!A22,"")</f>
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="str">
         <f>IF(timeseries!A23&lt;&gt;"",timeseries!A23,"")</f>
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="str">
         <f>IF(timeseries!A24&lt;&gt;"",timeseries!A24,"")</f>
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="str">
         <f>IF(timeseries!A25&lt;&gt;"",timeseries!A25,"")</f>
         <v/>
@@ -4516,7 +4580,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F87DD44-A1AD-4241-AED7-C48CC9DEE2E2}">
   <dimension ref="A1:G25"/>
   <sheetViews>
@@ -4524,14 +4588,14 @@
       <selection activeCell="H14" sqref="E1:H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.33203125" style="8" customWidth="1"/>
-    <col min="4" max="6" width="10.44140625" customWidth="1"/>
-    <col min="7" max="7" width="10.44140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" style="8" customWidth="1"/>
+    <col min="4" max="6" width="10.42578125" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>25</v>
       </c>
@@ -4542,7 +4606,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
         <f>IF(timeseries!A2&lt;&gt;"",timeseries!A2,"")</f>
         <v>44671</v>
@@ -4556,7 +4620,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <f>IF(timeseries!A3&lt;&gt;"",timeseries!A3,"")</f>
         <v>44671.041666666664</v>
@@ -4570,7 +4634,7 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <f>IF(timeseries!A4&lt;&gt;"",timeseries!A4,"")</f>
         <v>44671.08333321759</v>
@@ -4584,7 +4648,7 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <f>IF(timeseries!A5&lt;&gt;"",timeseries!A5,"")</f>
         <v>44671.124999826388</v>
@@ -4598,7 +4662,7 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <f>IF(timeseries!A6&lt;&gt;"",timeseries!A6,"")</f>
         <v>44671.166666435187</v>
@@ -4612,7 +4676,7 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <f>IF(timeseries!A7&lt;&gt;"",timeseries!A7,"")</f>
         <v>44671.208333043978</v>
@@ -4626,7 +4690,7 @@
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <f>IF(timeseries!A8&lt;&gt;"",timeseries!A8,"")</f>
         <v>44671.249999537038</v>
@@ -4640,7 +4704,7 @@
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <f>IF(timeseries!A9&lt;&gt;"",timeseries!A9,"")</f>
         <v>44671.291666087964</v>
@@ -4654,7 +4718,7 @@
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
         <f>IF(timeseries!A10&lt;&gt;"",timeseries!A10,"")</f>
         <v>44671.333332638889</v>
@@ -4668,7 +4732,7 @@
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <f>IF(timeseries!A11&lt;&gt;"",timeseries!A11,"")</f>
         <v>44671.374999189815</v>
@@ -4682,7 +4746,7 @@
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="str">
         <f>IF(timeseries!A12&lt;&gt;"",timeseries!A12,"")</f>
         <v/>
@@ -4690,7 +4754,7 @@
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="str">
         <f>IF(timeseries!A13&lt;&gt;"",timeseries!A13,"")</f>
         <v/>
@@ -4698,7 +4762,7 @@
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="str">
         <f>IF(timeseries!A14&lt;&gt;"",timeseries!A14,"")</f>
         <v/>
@@ -4706,7 +4770,7 @@
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="str">
         <f>IF(timeseries!A15&lt;&gt;"",timeseries!A15,"")</f>
         <v/>
@@ -4714,7 +4778,7 @@
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="str">
         <f>IF(timeseries!A16&lt;&gt;"",timeseries!A16,"")</f>
         <v/>
@@ -4722,7 +4786,7 @@
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="str">
         <f>IF(timeseries!A17&lt;&gt;"",timeseries!A17,"")</f>
         <v/>
@@ -4730,7 +4794,7 @@
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="str">
         <f>IF(timeseries!A18&lt;&gt;"",timeseries!A18,"")</f>
         <v/>
@@ -4738,7 +4802,7 @@
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="str">
         <f>IF(timeseries!A19&lt;&gt;"",timeseries!A19,"")</f>
         <v/>
@@ -4746,7 +4810,7 @@
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="str">
         <f>IF(timeseries!A20&lt;&gt;"",timeseries!A20,"")</f>
         <v/>
@@ -4754,7 +4818,7 @@
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="str">
         <f>IF(timeseries!A21&lt;&gt;"",timeseries!A21,"")</f>
         <v/>
@@ -4762,7 +4826,7 @@
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="str">
         <f>IF(timeseries!A22&lt;&gt;"",timeseries!A22,"")</f>
         <v/>
@@ -4770,7 +4834,7 @@
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="str">
         <f>IF(timeseries!A23&lt;&gt;"",timeseries!A23,"")</f>
         <v/>
@@ -4778,7 +4842,7 @@
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="str">
         <f>IF(timeseries!A24&lt;&gt;"",timeseries!A24,"")</f>
         <v/>
@@ -4786,7 +4850,7 @@
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="str">
         <f>IF(timeseries!A25&lt;&gt;"",timeseries!A25,"")</f>
         <v/>
@@ -4801,7 +4865,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E44A96C9-CA4B-4735-AF1E-65BD86DB3657}">
   <dimension ref="A1:F17"/>
   <sheetViews>
@@ -4809,82 +4873,82 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.6640625" customWidth="1"/>
+    <col min="3" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="C2" s="8"/>
       <c r="E2" s="8"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="C3" s="8"/>
       <c r="E3" s="8"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="C4" s="8"/>
       <c r="E4" s="8"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="C5" s="8"/>
       <c r="E5" s="8"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
       <c r="F15" s="8"/>
     </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
@@ -4895,7 +4959,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02307C1F-427B-487D-B703-EBF512D7AC27}">
   <dimension ref="A1:C25"/>
   <sheetViews>
@@ -4903,12 +4967,12 @@
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.33203125" style="8" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>25</v>
       </c>
@@ -4919,7 +4983,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
         <f>IF(timeseries!A2&lt;&gt;"",timeseries!A2,"")</f>
         <v>44671</v>
@@ -4931,7 +4995,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <f>IF(timeseries!A3&lt;&gt;"",timeseries!A3,"")</f>
         <v>44671.041666666664</v>
@@ -4943,7 +5007,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <f>IF(timeseries!A4&lt;&gt;"",timeseries!A4,"")</f>
         <v>44671.08333321759</v>
@@ -4955,7 +5019,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <f>IF(timeseries!A5&lt;&gt;"",timeseries!A5,"")</f>
         <v>44671.124999826388</v>
@@ -4967,7 +5031,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <f>IF(timeseries!A6&lt;&gt;"",timeseries!A6,"")</f>
         <v>44671.166666435187</v>
@@ -4979,7 +5043,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <f>IF(timeseries!A7&lt;&gt;"",timeseries!A7,"")</f>
         <v>44671.208333043978</v>
@@ -4991,7 +5055,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <f>IF(timeseries!A8&lt;&gt;"",timeseries!A8,"")</f>
         <v>44671.249999537038</v>
@@ -5003,7 +5067,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <f>IF(timeseries!A9&lt;&gt;"",timeseries!A9,"")</f>
         <v>44671.291666087964</v>
@@ -5015,7 +5079,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
         <f>IF(timeseries!A10&lt;&gt;"",timeseries!A10,"")</f>
         <v>44671.333332638889</v>
@@ -5027,7 +5091,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <f>IF(timeseries!A11&lt;&gt;"",timeseries!A11,"")</f>
         <v>44671.374999189815</v>
@@ -5039,85 +5103,85 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="str">
         <f>IF(timeseries!A12&lt;&gt;"",timeseries!A12,"")</f>
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="str">
         <f>IF(timeseries!A13&lt;&gt;"",timeseries!A13,"")</f>
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="str">
         <f>IF(timeseries!A14&lt;&gt;"",timeseries!A14,"")</f>
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="str">
         <f>IF(timeseries!A15&lt;&gt;"",timeseries!A15,"")</f>
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="str">
         <f>IF(timeseries!A16&lt;&gt;"",timeseries!A16,"")</f>
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="str">
         <f>IF(timeseries!A17&lt;&gt;"",timeseries!A17,"")</f>
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="str">
         <f>IF(timeseries!A18&lt;&gt;"",timeseries!A18,"")</f>
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="str">
         <f>IF(timeseries!A19&lt;&gt;"",timeseries!A19,"")</f>
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="str">
         <f>IF(timeseries!A20&lt;&gt;"",timeseries!A20,"")</f>
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="str">
         <f>IF(timeseries!A21&lt;&gt;"",timeseries!A21,"")</f>
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="str">
         <f>IF(timeseries!A22&lt;&gt;"",timeseries!A22,"")</f>
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="str">
         <f>IF(timeseries!A23&lt;&gt;"",timeseries!A23,"")</f>
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="str">
         <f>IF(timeseries!A24&lt;&gt;"",timeseries!A24,"")</f>
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="str">
         <f>IF(timeseries!A25&lt;&gt;"",timeseries!A25,"")</f>
         <v/>
@@ -5129,7 +5193,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3788A93-7501-4F5D-9E8F-38D329CC85EC}">
   <dimension ref="A1:L5"/>
   <sheetViews>
@@ -5137,19 +5201,19 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.5546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.88671875" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.33203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.44140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.109375" style="7"/>
+    <col min="2" max="2" width="7.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>26</v>
       </c>
@@ -5187,7 +5251,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>10</v>
       </c>
@@ -5225,7 +5289,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>61</v>
       </c>
@@ -5263,7 +5327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>80</v>
       </c>
@@ -5301,7 +5365,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I5"/>
     </row>
   </sheetData>
@@ -5309,7 +5373,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3E266E0-7523-413E-8B0C-F3E2413808A5}">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -5317,13 +5381,13 @@
       <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.44140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="6.5546875" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="6.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>98</v>
       </c>
@@ -5334,7 +5398,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>61</v>
       </c>
@@ -5345,7 +5409,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>80</v>
       </c>
@@ -5361,7 +5425,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF6DDD9A-EF34-4108-8532-230729E9C708}">
   <dimension ref="A1:G11"/>
   <sheetViews>
@@ -5369,14 +5433,14 @@
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.33203125" style="8" customWidth="1"/>
-    <col min="2" max="6" width="11.44140625" customWidth="1"/>
-    <col min="7" max="14" width="11.109375" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" style="8" customWidth="1"/>
+    <col min="2" max="6" width="11.42578125" customWidth="1"/>
+    <col min="7" max="14" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>25</v>
       </c>
@@ -5399,7 +5463,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
         <f>IF(timeseries!A2&lt;&gt;"",timeseries!A2,"")</f>
         <v>44671</v>
@@ -5423,7 +5487,7 @@
         <v>134.68</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <f>IF(timeseries!A3&lt;&gt;"",timeseries!A3,"")</f>
         <v>44671.041666666664</v>
@@ -5447,7 +5511,7 @@
         <v>271.23</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <f>IF(timeseries!A4&lt;&gt;"",timeseries!A4,"")</f>
         <v>44671.08333321759</v>
@@ -5471,7 +5535,7 @@
         <v>53.8</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <f>IF(timeseries!A5&lt;&gt;"",timeseries!A5,"")</f>
         <v>44671.124999826388</v>
@@ -5495,7 +5559,7 @@
         <v>220.9</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <f>IF(timeseries!A6&lt;&gt;"",timeseries!A6,"")</f>
         <v>44671.166666435187</v>
@@ -5519,7 +5583,7 @@
         <v>171.55</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <f>IF(timeseries!A7&lt;&gt;"",timeseries!A7,"")</f>
         <v>44671.208333043978</v>
@@ -5543,7 +5607,7 @@
         <v>397.42</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <f>IF(timeseries!A8&lt;&gt;"",timeseries!A8,"")</f>
         <v>44671.249999537038</v>
@@ -5567,7 +5631,7 @@
         <v>191.92</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <f>IF(timeseries!A9&lt;&gt;"",timeseries!A9,"")</f>
         <v>44671.291666087964</v>
@@ -5591,7 +5655,7 @@
         <v>265.85000000000002</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
         <f>IF(timeseries!A10&lt;&gt;"",timeseries!A10,"")</f>
         <v>44671.333332638889</v>
@@ -5615,7 +5679,7 @@
         <v>299.97000000000003</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <f>IF(timeseries!A11&lt;&gt;"",timeseries!A11,"")</f>
         <v>44671.374999189815</v>
@@ -5647,7 +5711,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{817FDE8F-BC70-48D0-8376-FB52E6946AF1}">
   <dimension ref="A1:E25"/>
   <sheetViews>
@@ -5655,14 +5719,14 @@
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>25</v>
       </c>
@@ -5679,7 +5743,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
         <f>IF(timeseries!A2&lt;&gt;"",timeseries!A2,"")</f>
         <v>44671</v>
@@ -5701,7 +5765,7 @@
         <v>14.933999999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <f>IF(timeseries!A3&lt;&gt;"",timeseries!A3,"")</f>
         <v>44671.041666666664</v>
@@ -5723,7 +5787,7 @@
         <v>6.7545000000000002</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <f>IF(timeseries!A4&lt;&gt;"",timeseries!A4,"")</f>
         <v>44671.08333321759</v>
@@ -5745,7 +5809,7 @@
         <v>34.6845</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <f>IF(timeseries!A5&lt;&gt;"",timeseries!A5,"")</f>
         <v>44671.124999826388</v>
@@ -5767,7 +5831,7 @@
         <v>26.847000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <f>IF(timeseries!A6&lt;&gt;"",timeseries!A6,"")</f>
         <v>44671.166666435187</v>
@@ -5789,7 +5853,7 @@
         <v>44.735500000000002</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <f>IF(timeseries!A7&lt;&gt;"",timeseries!A7,"")</f>
         <v>44671.208333043978</v>
@@ -5811,7 +5875,7 @@
         <v>31.805999999999994</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <f>IF(timeseries!A8&lt;&gt;"",timeseries!A8,"")</f>
         <v>44671.249999537038</v>
@@ -5833,7 +5897,7 @@
         <v>64.998999999999995</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <f>IF(timeseries!A9&lt;&gt;"",timeseries!A9,"")</f>
         <v>44671.291666087964</v>
@@ -5855,7 +5919,7 @@
         <v>61.474499999999992</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
         <f>IF(timeseries!A10&lt;&gt;"",timeseries!A10,"")</f>
         <v>44671.333332638889</v>
@@ -5877,7 +5941,7 @@
         <v>9.1009999999999991</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <f>IF(timeseries!A11&lt;&gt;"",timeseries!A11,"")</f>
         <v>44671.374999189815</v>
@@ -5899,50 +5963,50 @@
         <v>22.486499999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="8"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="8"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="8"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="8"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="8"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="8"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="8"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="8"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="8"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="8"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="8"/>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="8"/>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="8"/>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="8"/>
     </row>
   </sheetData>
@@ -5951,7 +6015,88 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5112C03D-AA3C-4BDB-99A8-E263BCF7A011}">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>117</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>119</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>120</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>121</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9314D326-256A-435C-AAE3-3517FA836EAE}">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -5959,12 +6104,12 @@
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>49</v>
       </c>
@@ -5972,7 +6117,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>51</v>
       </c>
@@ -5980,7 +6125,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>52</v>
       </c>
@@ -5993,221 +6138,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04A1B16B-CDA9-46BD-BA51-731AA9327652}">
-  <dimension ref="A1:O4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.6640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="7">
-        <v>1</v>
-      </c>
-      <c r="C2" s="7">
-        <v>0</v>
-      </c>
-      <c r="D2" s="7">
-        <v>0</v>
-      </c>
-      <c r="E2" s="7">
-        <v>0</v>
-      </c>
-      <c r="F2" s="7">
-        <v>0</v>
-      </c>
-      <c r="G2" s="7">
-        <v>0</v>
-      </c>
-      <c r="H2" s="7">
-        <v>0</v>
-      </c>
-      <c r="I2" s="7">
-        <v>0</v>
-      </c>
-      <c r="J2" s="7">
-        <v>0</v>
-      </c>
-      <c r="K2" s="7">
-        <v>0</v>
-      </c>
-      <c r="L2" s="7">
-        <v>0</v>
-      </c>
-      <c r="M2" s="7">
-        <v>0</v>
-      </c>
-      <c r="N2" s="7">
-        <v>0</v>
-      </c>
-      <c r="O2" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="7">
-        <v>0</v>
-      </c>
-      <c r="C3" s="7">
-        <v>0</v>
-      </c>
-      <c r="D3" s="7">
-        <v>1</v>
-      </c>
-      <c r="E3" s="7">
-        <v>0</v>
-      </c>
-      <c r="F3" s="7">
-        <v>0</v>
-      </c>
-      <c r="G3" s="7">
-        <v>0</v>
-      </c>
-      <c r="H3" s="7">
-        <v>0</v>
-      </c>
-      <c r="I3" s="7">
-        <v>0</v>
-      </c>
-      <c r="J3" s="7">
-        <v>0</v>
-      </c>
-      <c r="K3" s="7">
-        <v>0</v>
-      </c>
-      <c r="L3" s="7">
-        <v>0</v>
-      </c>
-      <c r="M3" s="7">
-        <v>0</v>
-      </c>
-      <c r="N3" s="7">
-        <v>0</v>
-      </c>
-      <c r="O3" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>72</v>
-      </c>
-      <c r="B4" s="7">
-        <v>0</v>
-      </c>
-      <c r="C4" s="7">
-        <v>0</v>
-      </c>
-      <c r="D4" s="7">
-        <v>0</v>
-      </c>
-      <c r="E4" s="7">
-        <v>0</v>
-      </c>
-      <c r="F4" s="7">
-        <v>1</v>
-      </c>
-      <c r="G4" s="7">
-        <v>0</v>
-      </c>
-      <c r="H4" s="7">
-        <v>0</v>
-      </c>
-      <c r="I4" s="7">
-        <v>0</v>
-      </c>
-      <c r="J4" s="7">
-        <v>0</v>
-      </c>
-      <c r="K4" s="7">
-        <v>0</v>
-      </c>
-      <c r="L4" s="7">
-        <v>0</v>
-      </c>
-      <c r="M4" s="7">
-        <v>0</v>
-      </c>
-      <c r="N4" s="7">
-        <v>0</v>
-      </c>
-      <c r="O4" s="7">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A87AD413-E614-48C1-80E1-F1E8236FCBC6}">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -6215,9 +6146,9 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>34</v>
       </c>
@@ -6225,7 +6156,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>36</v>
       </c>
@@ -6233,7 +6164,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>37</v>
       </c>
@@ -6246,7 +6177,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31679CA5-0AA2-4F6F-8223-14BF74917F04}">
   <dimension ref="A1:B25"/>
   <sheetViews>
@@ -6254,162 +6185,162 @@
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.33203125" style="8" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
         <f>IF(timeseries!A2&lt;&gt;"",timeseries!A2,"")</f>
         <v>44671</v>
       </c>
       <c r="B2" s="2"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <f>IF(timeseries!A3&lt;&gt;"",timeseries!A3,"")</f>
         <v>44671.041666666664</v>
       </c>
       <c r="B3" s="2"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <f>IF(timeseries!A4&lt;&gt;"",timeseries!A4,"")</f>
         <v>44671.08333321759</v>
       </c>
       <c r="B4" s="2"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <f>IF(timeseries!A5&lt;&gt;"",timeseries!A5,"")</f>
         <v>44671.124999826388</v>
       </c>
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <f>IF(timeseries!A6&lt;&gt;"",timeseries!A6,"")</f>
         <v>44671.166666435187</v>
       </c>
       <c r="B6" s="2"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <f>IF(timeseries!A7&lt;&gt;"",timeseries!A7,"")</f>
         <v>44671.208333043978</v>
       </c>
       <c r="B7" s="2"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <f>IF(timeseries!A8&lt;&gt;"",timeseries!A8,"")</f>
         <v>44671.249999537038</v>
       </c>
       <c r="B8" s="2"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <f>IF(timeseries!A9&lt;&gt;"",timeseries!A9,"")</f>
         <v>44671.291666087964</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
         <f>IF(timeseries!A10&lt;&gt;"",timeseries!A10,"")</f>
         <v>44671.333332638889</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <f>IF(timeseries!A11&lt;&gt;"",timeseries!A11,"")</f>
         <v>44671.374999189815</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="str">
         <f>IF(timeseries!A12&lt;&gt;"",timeseries!A12,"")</f>
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="str">
         <f>IF(timeseries!A13&lt;&gt;"",timeseries!A13,"")</f>
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="str">
         <f>IF(timeseries!A14&lt;&gt;"",timeseries!A14,"")</f>
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="str">
         <f>IF(timeseries!A15&lt;&gt;"",timeseries!A15,"")</f>
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="str">
         <f>IF(timeseries!A16&lt;&gt;"",timeseries!A16,"")</f>
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="str">
         <f>IF(timeseries!A17&lt;&gt;"",timeseries!A17,"")</f>
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="str">
         <f>IF(timeseries!A18&lt;&gt;"",timeseries!A18,"")</f>
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="str">
         <f>IF(timeseries!A19&lt;&gt;"",timeseries!A19,"")</f>
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="str">
         <f>IF(timeseries!A20&lt;&gt;"",timeseries!A20,"")</f>
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="str">
         <f>IF(timeseries!A21&lt;&gt;"",timeseries!A21,"")</f>
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="str">
         <f>IF(timeseries!A22&lt;&gt;"",timeseries!A22,"")</f>
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="str">
         <f>IF(timeseries!A23&lt;&gt;"",timeseries!A23,"")</f>
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="str">
         <f>IF(timeseries!A24&lt;&gt;"",timeseries!A24,"")</f>
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="str">
         <f>IF(timeseries!A25&lt;&gt;"",timeseries!A25,"")</f>
         <v/>
@@ -6420,7 +6351,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD670E02-665B-45B8-BC4E-9596D2C1BC55}">
   <dimension ref="A1:A25"/>
   <sheetViews>
@@ -6428,155 +6359,155 @@
       <selection activeCell="B1" sqref="B1:D1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.33203125" style="8" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
         <f>IF(timeseries!A2&lt;&gt;"",timeseries!A2,"")</f>
         <v>44671</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <f>IF(timeseries!A3&lt;&gt;"",timeseries!A3,"")</f>
         <v>44671.041666666664</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <f>IF(timeseries!A4&lt;&gt;"",timeseries!A4,"")</f>
         <v>44671.08333321759</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <f>IF(timeseries!A5&lt;&gt;"",timeseries!A5,"")</f>
         <v>44671.124999826388</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <f>IF(timeseries!A6&lt;&gt;"",timeseries!A6,"")</f>
         <v>44671.166666435187</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <f>IF(timeseries!A7&lt;&gt;"",timeseries!A7,"")</f>
         <v>44671.208333043978</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <f>IF(timeseries!A8&lt;&gt;"",timeseries!A8,"")</f>
         <v>44671.249999537038</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <f>IF(timeseries!A9&lt;&gt;"",timeseries!A9,"")</f>
         <v>44671.291666087964</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
         <f>IF(timeseries!A10&lt;&gt;"",timeseries!A10,"")</f>
         <v>44671.333332638889</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <f>IF(timeseries!A11&lt;&gt;"",timeseries!A11,"")</f>
         <v>44671.374999189815</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="str">
         <f>IF(timeseries!A12&lt;&gt;"",timeseries!A12,"")</f>
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="str">
         <f>IF(timeseries!A13&lt;&gt;"",timeseries!A13,"")</f>
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="str">
         <f>IF(timeseries!A14&lt;&gt;"",timeseries!A14,"")</f>
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="str">
         <f>IF(timeseries!A15&lt;&gt;"",timeseries!A15,"")</f>
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="str">
         <f>IF(timeseries!A16&lt;&gt;"",timeseries!A16,"")</f>
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="str">
         <f>IF(timeseries!A17&lt;&gt;"",timeseries!A17,"")</f>
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="str">
         <f>IF(timeseries!A18&lt;&gt;"",timeseries!A18,"")</f>
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="str">
         <f>IF(timeseries!A19&lt;&gt;"",timeseries!A19,"")</f>
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="str">
         <f>IF(timeseries!A20&lt;&gt;"",timeseries!A20,"")</f>
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="str">
         <f>IF(timeseries!A21&lt;&gt;"",timeseries!A21,"")</f>
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="str">
         <f>IF(timeseries!A22&lt;&gt;"",timeseries!A22,"")</f>
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="str">
         <f>IF(timeseries!A23&lt;&gt;"",timeseries!A23,"")</f>
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="str">
         <f>IF(timeseries!A24&lt;&gt;"",timeseries!A24,"")</f>
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="str">
         <f>IF(timeseries!A25&lt;&gt;"",timeseries!A25,"")</f>
         <v/>
@@ -6588,7 +6519,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7FEDBA5-B0F3-4E9D-9367-08D5F5FA8AEA}">
   <dimension ref="A1:A25"/>
   <sheetViews>
@@ -6596,155 +6527,155 @@
       <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.33203125" style="8" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
         <f>IF(timeseries!A2&lt;&gt;"",timeseries!A2,"")</f>
         <v>44671</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <f>IF(timeseries!A3&lt;&gt;"",timeseries!A3,"")</f>
         <v>44671.041666666664</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <f>IF(timeseries!A4&lt;&gt;"",timeseries!A4,"")</f>
         <v>44671.08333321759</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <f>IF(timeseries!A5&lt;&gt;"",timeseries!A5,"")</f>
         <v>44671.124999826388</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <f>IF(timeseries!A6&lt;&gt;"",timeseries!A6,"")</f>
         <v>44671.166666435187</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <f>IF(timeseries!A7&lt;&gt;"",timeseries!A7,"")</f>
         <v>44671.208333043978</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <f>IF(timeseries!A8&lt;&gt;"",timeseries!A8,"")</f>
         <v>44671.249999537038</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <f>IF(timeseries!A9&lt;&gt;"",timeseries!A9,"")</f>
         <v>44671.291666087964</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
         <f>IF(timeseries!A10&lt;&gt;"",timeseries!A10,"")</f>
         <v>44671.333332638889</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <f>IF(timeseries!A11&lt;&gt;"",timeseries!A11,"")</f>
         <v>44671.374999189815</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="str">
         <f>IF(timeseries!A12&lt;&gt;"",timeseries!A12,"")</f>
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="str">
         <f>IF(timeseries!A13&lt;&gt;"",timeseries!A13,"")</f>
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="str">
         <f>IF(timeseries!A14&lt;&gt;"",timeseries!A14,"")</f>
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="str">
         <f>IF(timeseries!A15&lt;&gt;"",timeseries!A15,"")</f>
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="str">
         <f>IF(timeseries!A16&lt;&gt;"",timeseries!A16,"")</f>
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="str">
         <f>IF(timeseries!A17&lt;&gt;"",timeseries!A17,"")</f>
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="str">
         <f>IF(timeseries!A18&lt;&gt;"",timeseries!A18,"")</f>
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="str">
         <f>IF(timeseries!A19&lt;&gt;"",timeseries!A19,"")</f>
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="str">
         <f>IF(timeseries!A20&lt;&gt;"",timeseries!A20,"")</f>
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="str">
         <f>IF(timeseries!A21&lt;&gt;"",timeseries!A21,"")</f>
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="str">
         <f>IF(timeseries!A22&lt;&gt;"",timeseries!A22,"")</f>
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="str">
         <f>IF(timeseries!A23&lt;&gt;"",timeseries!A23,"")</f>
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="str">
         <f>IF(timeseries!A24&lt;&gt;"",timeseries!A24,"")</f>
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="str">
         <f>IF(timeseries!A25&lt;&gt;"",timeseries!A25,"")</f>
         <v/>
@@ -6755,7 +6686,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5704FC51-737E-45F9-9A9E-85A96AFE5439}">
   <dimension ref="A1:M9"/>
   <sheetViews>
@@ -6763,14 +6694,14 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>34</v>
       </c>
@@ -6784,7 +6715,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>84</v>
       </c>
@@ -6798,7 +6729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
@@ -6809,7 +6740,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE12AB76-2BDA-4ACA-A128-8CFB9FB6C8F8}">
   <dimension ref="A1:G25"/>
   <sheetViews>
@@ -6817,15 +6748,15 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.33203125" style="8" customWidth="1"/>
-    <col min="2" max="4" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" style="8" customWidth="1"/>
+    <col min="2" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="5.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>25</v>
       </c>
@@ -6848,7 +6779,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
         <f>IF(timeseries!A2&lt;&gt;"",timeseries!A2,"")</f>
         <v>44671</v>
@@ -6872,7 +6803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <f>IF(timeseries!A3&lt;&gt;"",timeseries!A3,"")</f>
         <v>44671.041666666664</v>
@@ -6896,7 +6827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <f>IF(timeseries!A4&lt;&gt;"",timeseries!A4,"")</f>
         <v>44671.08333321759</v>
@@ -6920,7 +6851,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <f>IF(timeseries!A5&lt;&gt;"",timeseries!A5,"")</f>
         <v>44671.124999826388</v>
@@ -6944,7 +6875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <f>IF(timeseries!A6&lt;&gt;"",timeseries!A6,"")</f>
         <v>44671.166666435187</v>
@@ -6968,7 +6899,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <f>IF(timeseries!A7&lt;&gt;"",timeseries!A7,"")</f>
         <v>44671.208333043978</v>
@@ -6992,7 +6923,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <f>IF(timeseries!A8&lt;&gt;"",timeseries!A8,"")</f>
         <v>44671.249999537038</v>
@@ -7016,7 +6947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <f>IF(timeseries!A9&lt;&gt;"",timeseries!A9,"")</f>
         <v>44671.291666087964</v>
@@ -7040,7 +6971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
         <f>IF(timeseries!A10&lt;&gt;"",timeseries!A10,"")</f>
         <v>44671.333332638889</v>
@@ -7064,7 +6995,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <f>IF(timeseries!A11&lt;&gt;"",timeseries!A11,"")</f>
         <v>44671.374999189815</v>
@@ -7088,85 +7019,85 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="str">
         <f>IF(timeseries!A12&lt;&gt;"",timeseries!A12,"")</f>
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="str">
         <f>IF(timeseries!A13&lt;&gt;"",timeseries!A13,"")</f>
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="str">
         <f>IF(timeseries!A14&lt;&gt;"",timeseries!A14,"")</f>
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="str">
         <f>IF(timeseries!A15&lt;&gt;"",timeseries!A15,"")</f>
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="str">
         <f>IF(timeseries!A16&lt;&gt;"",timeseries!A16,"")</f>
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="str">
         <f>IF(timeseries!A17&lt;&gt;"",timeseries!A17,"")</f>
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="str">
         <f>IF(timeseries!A18&lt;&gt;"",timeseries!A18,"")</f>
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="str">
         <f>IF(timeseries!A19&lt;&gt;"",timeseries!A19,"")</f>
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="str">
         <f>IF(timeseries!A20&lt;&gt;"",timeseries!A20,"")</f>
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="str">
         <f>IF(timeseries!A21&lt;&gt;"",timeseries!A21,"")</f>
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="str">
         <f>IF(timeseries!A22&lt;&gt;"",timeseries!A22,"")</f>
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="str">
         <f>IF(timeseries!A23&lt;&gt;"",timeseries!A23,"")</f>
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="str">
         <f>IF(timeseries!A24&lt;&gt;"",timeseries!A24,"")</f>
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="str">
         <f>IF(timeseries!A25&lt;&gt;"",timeseries!A25,"")</f>
         <v/>
@@ -7178,155 +7109,153 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB20090B-02A9-43B7-8D03-9C18D42920EB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04A1B16B-CDA9-46BD-BA51-731AA9327652}">
   <dimension ref="A1:P4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.6640625" customWidth="1"/>
-    <col min="7" max="7" width="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="11.44140625" customWidth="1"/>
+    <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>46</v>
+        <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>18</v>
+        <v>105</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>38</v>
+        <v>5</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>68</v>
+        <v>114</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>69</v>
+        <v>106</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>47</v>
+        <v>107</v>
       </c>
       <c r="P1" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>73</v>
+        <v>7</v>
       </c>
       <c r="B2" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2" s="7">
         <v>0</v>
       </c>
       <c r="D2" s="7">
+        <v>0</v>
+      </c>
+      <c r="E2" s="7">
+        <v>0</v>
+      </c>
+      <c r="F2" s="7">
+        <v>0</v>
+      </c>
+      <c r="G2" s="7">
+        <v>0</v>
+      </c>
+      <c r="H2" s="7">
+        <v>0</v>
+      </c>
+      <c r="I2" s="7">
+        <v>0</v>
+      </c>
+      <c r="J2" s="7">
+        <v>0</v>
+      </c>
+      <c r="K2" s="7">
+        <v>0</v>
+      </c>
+      <c r="L2" s="7">
+        <v>0</v>
+      </c>
+      <c r="M2" s="7">
+        <v>0</v>
+      </c>
+      <c r="N2" s="7">
+        <v>0</v>
+      </c>
+      <c r="O2" s="7">
+        <v>0</v>
+      </c>
+      <c r="P2" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="7">
+        <v>0</v>
+      </c>
+      <c r="C3" s="7">
+        <v>0</v>
+      </c>
+      <c r="D3" s="7">
         <v>1</v>
       </c>
-      <c r="E2" s="7">
-        <v>1</v>
-      </c>
-      <c r="F2" s="7">
-        <v>1</v>
-      </c>
-      <c r="G2" s="7">
-        <v>0.9</v>
-      </c>
-      <c r="H2" s="7">
-        <v>0.3</v>
-      </c>
-      <c r="I2" s="7">
-        <v>1</v>
-      </c>
-      <c r="J2" s="7">
-        <v>1</v>
-      </c>
-      <c r="K2" s="7">
-        <v>2</v>
-      </c>
-      <c r="L2" s="7">
-        <v>2</v>
-      </c>
-      <c r="M2" s="7">
-        <v>0</v>
-      </c>
-      <c r="N2" s="7">
-        <v>0</v>
-      </c>
-      <c r="O2" s="7">
-        <v>1</v>
-      </c>
-      <c r="P2" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>75</v>
-      </c>
-      <c r="B3" s="7">
-        <v>1</v>
-      </c>
-      <c r="C3" s="7">
-        <v>0</v>
-      </c>
-      <c r="D3" s="7">
-        <v>0</v>
-      </c>
       <c r="E3" s="7">
         <v>0</v>
       </c>
       <c r="F3" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G3" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H3" s="7">
         <v>0</v>
       </c>
       <c r="I3" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J3" s="7">
         <v>0</v>
@@ -7350,9 +7279,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B4" s="7">
         <v>0</v>
@@ -7364,19 +7293,19 @@
         <v>0</v>
       </c>
       <c r="E4" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4" s="7">
         <v>1</v>
       </c>
       <c r="G4" s="7">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H4" s="7">
         <v>0</v>
       </c>
       <c r="I4" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J4" s="7">
         <v>0</v>
@@ -7406,6 +7335,249 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB20090B-02A9-43B7-8D03-9C18D42920EB}">
+  <dimension ref="A1:Q9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q10" sqref="Q10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" customWidth="1"/>
+    <col min="7" max="7" width="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="11.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2" s="7">
+        <v>0</v>
+      </c>
+      <c r="C2" s="7">
+        <v>0</v>
+      </c>
+      <c r="D2" s="7">
+        <v>1</v>
+      </c>
+      <c r="E2" s="7">
+        <v>1</v>
+      </c>
+      <c r="F2" s="7">
+        <v>1</v>
+      </c>
+      <c r="G2" s="7">
+        <v>0.9</v>
+      </c>
+      <c r="H2" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="I2" s="7">
+        <v>1</v>
+      </c>
+      <c r="J2" s="7">
+        <v>1</v>
+      </c>
+      <c r="K2" s="7">
+        <v>2</v>
+      </c>
+      <c r="L2" s="7">
+        <v>2</v>
+      </c>
+      <c r="M2" s="7">
+        <v>0</v>
+      </c>
+      <c r="N2" s="7">
+        <v>0</v>
+      </c>
+      <c r="O2" s="7">
+        <v>1</v>
+      </c>
+      <c r="P2" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3" s="7">
+        <v>1</v>
+      </c>
+      <c r="C3" s="7">
+        <v>0</v>
+      </c>
+      <c r="D3" s="7">
+        <v>0</v>
+      </c>
+      <c r="E3" s="7">
+        <v>0</v>
+      </c>
+      <c r="F3" s="7">
+        <v>1</v>
+      </c>
+      <c r="G3" s="7">
+        <v>1</v>
+      </c>
+      <c r="H3" s="7">
+        <v>0</v>
+      </c>
+      <c r="I3" s="7">
+        <v>1</v>
+      </c>
+      <c r="J3" s="7">
+        <v>0</v>
+      </c>
+      <c r="K3" s="7">
+        <v>0</v>
+      </c>
+      <c r="L3" s="7">
+        <v>0</v>
+      </c>
+      <c r="M3" s="7">
+        <v>0</v>
+      </c>
+      <c r="N3" s="7">
+        <v>0</v>
+      </c>
+      <c r="O3" s="7">
+        <v>0</v>
+      </c>
+      <c r="P3" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" s="7">
+        <v>0</v>
+      </c>
+      <c r="C4" s="7">
+        <v>0</v>
+      </c>
+      <c r="D4" s="7">
+        <v>0</v>
+      </c>
+      <c r="E4" s="7">
+        <v>1</v>
+      </c>
+      <c r="F4" s="7">
+        <v>1</v>
+      </c>
+      <c r="G4" s="7">
+        <v>3</v>
+      </c>
+      <c r="H4" s="7">
+        <v>0</v>
+      </c>
+      <c r="I4" s="7">
+        <v>1</v>
+      </c>
+      <c r="J4" s="7">
+        <v>0</v>
+      </c>
+      <c r="K4" s="7">
+        <v>0</v>
+      </c>
+      <c r="L4" s="7">
+        <v>0</v>
+      </c>
+      <c r="M4" s="7">
+        <v>0</v>
+      </c>
+      <c r="N4" s="7">
+        <v>0</v>
+      </c>
+      <c r="O4" s="7">
+        <v>0</v>
+      </c>
+      <c r="P4" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q9" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5539A729-4FB7-440D-A765-676495DE3453}">
   <dimension ref="A1:C4"/>
   <sheetViews>
@@ -7413,9 +7585,9 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>30</v>
       </c>
@@ -7426,7 +7598,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -7437,7 +7609,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -7448,7 +7620,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -7464,7 +7636,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAB1106B-D567-41FC-8E91-2B4CC5EC9B59}">
   <dimension ref="A1:K1"/>
   <sheetViews>
@@ -7472,9 +7644,9 @@
       <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>11</v>
       </c>
@@ -7523,28 +7695,28 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A86A8A7-FD76-4891-A53C-CBB095359118}">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.88671875" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.44140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.5546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.44140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.88671875" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.5546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.109375" style="5"/>
+    <col min="1" max="1" width="16.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>11</v>
       </c>
@@ -7569,8 +7741,14 @@
       <c r="H1" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I1" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>73</v>
       </c>
@@ -7595,8 +7773,14 @@
       <c r="H2" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I2" s="5">
+        <v>0.7</v>
+      </c>
+      <c r="J2" s="5">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>73</v>
       </c>
@@ -7621,8 +7805,14 @@
       <c r="H3" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I3" s="5">
+        <v>0.7</v>
+      </c>
+      <c r="J3" s="5">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>73</v>
       </c>
@@ -7647,8 +7837,14 @@
       <c r="H4" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I4" s="5">
+        <v>0.7</v>
+      </c>
+      <c r="J4" s="5">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>75</v>
       </c>
@@ -7673,8 +7869,14 @@
       <c r="H5" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I5" s="5">
+        <v>0.7</v>
+      </c>
+      <c r="J5" s="5">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>74</v>
       </c>
@@ -7699,8 +7901,14 @@
       <c r="H6" s="5">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I6" s="5">
+        <v>0.7</v>
+      </c>
+      <c r="J6" s="5">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>74</v>
       </c>
@@ -7725,11 +7933,17 @@
       <c r="H7" s="5">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I7" s="5">
+        <v>0.7</v>
+      </c>
+      <c r="J7" s="5">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9"/>
     </row>
   </sheetData>
@@ -7738,7 +7952,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7AEF404-3743-47D7-AC45-7AE3A9FB796E}">
   <dimension ref="A1:A25"/>
   <sheetViews>
@@ -7746,155 +7960,155 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.33203125" style="8" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
         <f>IF(timeseries!A2&lt;&gt;"",timeseries!A2,"")</f>
         <v>44671</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <f>IF(timeseries!A3&lt;&gt;"",timeseries!A3,"")</f>
         <v>44671.041666666664</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <f>IF(timeseries!A4&lt;&gt;"",timeseries!A4,"")</f>
         <v>44671.08333321759</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <f>IF(timeseries!A5&lt;&gt;"",timeseries!A5,"")</f>
         <v>44671.124999826388</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <f>IF(timeseries!A6&lt;&gt;"",timeseries!A6,"")</f>
         <v>44671.166666435187</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <f>IF(timeseries!A7&lt;&gt;"",timeseries!A7,"")</f>
         <v>44671.208333043978</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <f>IF(timeseries!A8&lt;&gt;"",timeseries!A8,"")</f>
         <v>44671.249999537038</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <f>IF(timeseries!A9&lt;&gt;"",timeseries!A9,"")</f>
         <v>44671.291666087964</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
         <f>IF(timeseries!A10&lt;&gt;"",timeseries!A10,"")</f>
         <v>44671.333332638889</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <f>IF(timeseries!A11&lt;&gt;"",timeseries!A11,"")</f>
         <v>44671.374999189815</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="str">
         <f>IF(timeseries!A12&lt;&gt;"",timeseries!A12,"")</f>
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="str">
         <f>IF(timeseries!A13&lt;&gt;"",timeseries!A13,"")</f>
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="str">
         <f>IF(timeseries!A14&lt;&gt;"",timeseries!A14,"")</f>
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="str">
         <f>IF(timeseries!A15&lt;&gt;"",timeseries!A15,"")</f>
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="str">
         <f>IF(timeseries!A16&lt;&gt;"",timeseries!A16,"")</f>
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="str">
         <f>IF(timeseries!A17&lt;&gt;"",timeseries!A17,"")</f>
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="str">
         <f>IF(timeseries!A18&lt;&gt;"",timeseries!A18,"")</f>
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="str">
         <f>IF(timeseries!A19&lt;&gt;"",timeseries!A19,"")</f>
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="str">
         <f>IF(timeseries!A20&lt;&gt;"",timeseries!A20,"")</f>
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="str">
         <f>IF(timeseries!A21&lt;&gt;"",timeseries!A21,"")</f>
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="str">
         <f>IF(timeseries!A22&lt;&gt;"",timeseries!A22,"")</f>
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="str">
         <f>IF(timeseries!A23&lt;&gt;"",timeseries!A23,"")</f>
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="str">
         <f>IF(timeseries!A24&lt;&gt;"",timeseries!A24,"")</f>
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="str">
         <f>IF(timeseries!A25&lt;&gt;"",timeseries!A25,"")</f>
         <v/>
@@ -7905,22 +8119,22 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{596E3FE2-967D-4C0B-BDAC-EF3704EC4DDF}">
   <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>102</v>
       </c>
@@ -7935,36 +8149,6 @@
       </c>
       <c r="E1" s="3" t="s">
         <v>110</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8F1FEF7-A337-4ADD-8F2A-03D982D23844}">
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="9.88671875" style="8" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>